<commit_message>
rename script.js to checklistScript.js
</commit_message>
<xml_diff>
--- a/public/games/hello-kitty-island-adventure/hello-kitty-island-adventure_data.xlsx
+++ b/public/games/hello-kitty-island-adventure/hello-kitty-island-adventure_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubChelsea\Achievement-Vault\public\games\hello-kitty-island-adventure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7880D7DE-1BAD-425D-A6F0-7FD0701CDE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF432354-5FC1-4FD1-8F48-CBF398714B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{EDF2BE8D-03F7-4EE0-AD1E-08AEE49FD7D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EDF2BE8D-03F7-4EE0-AD1E-08AEE49FD7D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4724,9 +4724,6 @@
   </cellStyles>
   <dxfs count="25">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -4805,6 +4802,9 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -5020,7 +5020,7 @@
     <tableColumn id="8" xr3:uid="{B87D96DA-876B-4321-974C-D3CA18927D46}" name="3-Heart Gifts"/>
     <tableColumn id="9" xr3:uid="{A8FFB3A6-3D98-46C6-9DA5-7615BB78E8C5}" name="2-Heart Gifts"/>
     <tableColumn id="10" xr3:uid="{2EF34846-880B-4FE1-BEBA-4EA7E502EABA}" name="1-Heart Gifts"/>
-    <tableColumn id="12" xr3:uid="{6D0FA26C-9E5B-468D-AD99-073C14547B04}" name="Description" dataDxfId="0">
+    <tableColumn id="12" xr3:uid="{6D0FA26C-9E5B-468D-AD99-073C14547B04}" name="Description" dataDxfId="8">
       <calculatedColumnFormula xml:space="preserve"> "Liked Gifts: " &amp; Table5[[#This Row],[Liked Gifts]] &amp; " /// 3-Heart Gifts: " &amp; Table5[[#This Row],[3-Heart Gifts]] &amp; " /// 2-Heart Gifts: " &amp; Table5[[#This Row],[2-Heart Gifts]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5347,8 +5347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B082B9-00AC-4E0F-A853-52691B39AEB7}">
   <dimension ref="A1:CJ62"/>
   <sheetViews>
-    <sheetView topLeftCell="BV1" workbookViewId="0">
-      <selection activeCell="CD2" sqref="CD2"/>
+    <sheetView tabSelected="1" topLeftCell="BV1" workbookViewId="0">
+      <selection activeCell="CB10" sqref="CB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12478,8 +12478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30E60DA8-4CCF-4656-AD01-A1646335A0A7}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G23"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13144,8 +13144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4FD85B-59D8-4D29-B4AF-8683988B5507}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14762,8 +14762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E0F9F24-98FF-4930-82DA-5BF13106EE36}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16382,8 +16382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB14B9A7-32BD-458D-A5F7-E49A0C0475BC}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16899,32 +16899,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:F3 A4:E4 A5:F21">
-    <cfRule type="containsText" dxfId="8" priority="9" stopIfTrue="1" operator="containsText" text="Tea Leaves">
-      <formula>NOT(ISERROR(SEARCH("Tea Leaves",A2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" stopIfTrue="1" operator="containsText" text="Tapioca">
-      <formula>NOT(ISERROR(SEARCH("Tapioca",A2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="11" stopIfTrue="1" operator="containsText" text="Starfruit">
-      <formula>NOT(ISERROR(SEARCH("Starfruit",A2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="12" stopIfTrue="1" operator="containsText" text="SnowCicle">
-      <formula>NOT(ISERROR(SEARCH("SnowCicle",A2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="13" stopIfTrue="1" operator="containsText" text="Bubble">
-      <formula>NOT(ISERROR(SEARCH("Bubble",A2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="14" stopIfTrue="1" operator="containsText" text="Sakura">
-      <formula>NOT(ISERROR(SEARCH("Sakura",A2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="15" stopIfTrue="1" operator="containsText" text="Egg">
-      <formula>NOT(ISERROR(SEARCH("Egg",A2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="16" stopIfTrue="1" operator="containsText" text="Moon Cheese">
-      <formula>NOT(ISERROR(SEARCH("Moon Cheese",A2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
update records, fix cozy grove landing page
</commit_message>
<xml_diff>
--- a/public/games/hello-kitty-island-adventure/hello-kitty-island-adventure_data.xlsx
+++ b/public/games/hello-kitty-island-adventure/hello-kitty-island-adventure_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubChelsea\Achievement-Vault\public\games\hello-kitty-island-adventure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF432354-5FC1-4FD1-8F48-CBF398714B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BABA97-284A-490A-8C37-ED79E63D70F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EDF2BE8D-03F7-4EE0-AD1E-08AEE49FD7D6}"/>
+    <workbookView xWindow="2535" yWindow="1950" windowWidth="21600" windowHeight="12525" xr2:uid="{EDF2BE8D-03F7-4EE0-AD1E-08AEE49FD7D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2211" uniqueCount="1533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2212" uniqueCount="1534">
   <si>
     <t>General Achievements</t>
   </si>
@@ -3775,9 +3775,6 @@
     <t>01 Seaside Resort - Sunslime</t>
   </si>
   <si>
-    <t>01 Seaside Resort - Victor Island Chase</t>
-  </si>
-  <si>
     <t>02 Spooky Swamp - Bottomless Bouldering</t>
   </si>
   <si>
@@ -4640,6 +4637,12 @@
   </si>
   <si>
     <t>Liked Gifts: Stars, Dreamy, Frozen /// 3-Heart Gifts: Starry Skies Shake /// 2-Heart Gifts: Art supplies, dreamy star</t>
+  </si>
+  <si>
+    <t>01 Seaside Resort - Visitor Island Chase</t>
+  </si>
+  <si>
+    <t>Double-check the #</t>
   </si>
 </sst>
 </file>
@@ -4669,7 +4672,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4694,6 +4697,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4707,7 +4716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4718,94 +4727,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -4924,6 +4851,9 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4946,10 +4876,10 @@
     <tableColumn id="3" xr3:uid="{67BA542E-A92B-464D-9C55-15FD3BA24444}" name="Location"/>
     <tableColumn id="4" xr3:uid="{8144ACCD-B001-4F9D-B87C-6C497C658DFE}" name="Item/Decor Requirements"/>
     <tableColumn id="5" xr3:uid="{57F66957-D073-4581-9F70-8D34A88575FD}" name="Daily Gift"/>
-    <tableColumn id="6" xr3:uid="{537E9DCC-239F-4D35-BCE6-8CB9BFB45223}" name="Description with Line Breaks" dataDxfId="24">
+    <tableColumn id="6" xr3:uid="{537E9DCC-239F-4D35-BCE6-8CB9BFB45223}" name="Description with Line Breaks" dataDxfId="16">
       <calculatedColumnFormula xml:space="preserve"> "Schedule: " &amp; Table1[[#This Row],[Visiting Schedule]] &amp; CHAR(10) &amp; "Location: " &amp; Table1[[#This Row],[Location]] &amp; CHAR(10) &amp; "Item/Decor Requirements: " &amp; Table1[[#This Row],[Item/Decor Requirements]] &amp; CHAR(10) &amp; "Daily Gift: " &amp; Table1[[#This Row],[Daily Gift]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E50BEB41-434D-4EDF-814B-0A977903EEA3}" name="Description without Line Breaks" dataDxfId="23">
+    <tableColumn id="7" xr3:uid="{E50BEB41-434D-4EDF-814B-0A977903EEA3}" name="Description without Line Breaks" dataDxfId="15">
       <calculatedColumnFormula xml:space="preserve"> "Schedule: " &amp; Table1[[#This Row],[Visiting Schedule]] &amp; " /// Location: " &amp; Table1[[#This Row],[Location]] &amp; " /// Item Requirements: " &amp; Table1[[#This Row],[Item/Decor Requirements]] &amp; " /// Daily Gift: " &amp; Table1[[#This Row],[Daily Gift]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4968,13 +4898,13 @@
     <tableColumn id="8" xr3:uid="{7C1C2515-B9D8-45FE-9359-EA852AF05641}" name="Column1"/>
     <tableColumn id="1" xr3:uid="{380CE29E-A949-4954-B10D-CBB92EBE432A}" name="Region"/>
     <tableColumn id="2" xr3:uid="{F8A98686-C2B1-4D72-8EE6-3DFA85AFF688}" name="Fish"/>
-    <tableColumn id="6" xr3:uid="{18B2DD51-2A8F-46E2-B608-19A620E07545}" name="Name" dataDxfId="22">
+    <tableColumn id="6" xr3:uid="{18B2DD51-2A8F-46E2-B608-19A620E07545}" name="Name" dataDxfId="14">
       <calculatedColumnFormula>Tbl_Fishing[[#This Row],[Region]] &amp; " - " &amp; Tbl_Fishing[[#This Row],[Fish]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{6EE718AE-717B-450F-AB60-68A1FC341603}" name="Location"/>
     <tableColumn id="4" xr3:uid="{F9636F26-A4D9-495A-B262-03386101172F}" name="Time"/>
     <tableColumn id="5" xr3:uid="{72995A89-7D21-4A08-BD4C-048FF0E81A79}" name="Rarity"/>
-    <tableColumn id="7" xr3:uid="{3AD6DEA4-0FD9-49BB-A6C1-7138C775149E}" name="Description" dataDxfId="21">
+    <tableColumn id="7" xr3:uid="{3AD6DEA4-0FD9-49BB-A6C1-7138C775149E}" name="Description" dataDxfId="13">
       <calculatedColumnFormula>"RARITY: " &amp; Tbl_Fishing[[#This Row],[Rarity]] &amp; " /// TIME: " &amp; Tbl_Fishing[[#This Row],[Time]] &amp; " /// LOCATION: " &amp; Tbl_Fishing[[#This Row],[Location]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4993,13 +4923,13 @@
     <tableColumn id="6" xr3:uid="{04674BA7-561C-43B4-AA53-702B0A90F402}" name="Region Order"/>
     <tableColumn id="1" xr3:uid="{91CAD11C-382E-4DF9-A2FD-BE370A57103A}" name="Region"/>
     <tableColumn id="2" xr3:uid="{24D43D77-F696-4AC9-9938-3DFE01D62DB9}" name="Critter"/>
-    <tableColumn id="7" xr3:uid="{F9762BCC-B476-49DF-A0F9-ACAB1857886B}" name="Name" dataDxfId="20">
+    <tableColumn id="7" xr3:uid="{F9762BCC-B476-49DF-A0F9-ACAB1857886B}" name="Name" dataDxfId="12">
       <calculatedColumnFormula>Table3[[#This Row],[Region]] &amp; " - " &amp; Table3[[#This Row],[Critter]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{1D57E4B8-C021-4B34-9B8B-8DAA071BC910}" name="Location"/>
     <tableColumn id="4" xr3:uid="{527DF911-157E-429B-B380-A788D97C284C}" name="Time"/>
     <tableColumn id="5" xr3:uid="{C5047F6F-39E5-4CEC-B7D7-BF773933D03C}" name="Rarity"/>
-    <tableColumn id="8" xr3:uid="{2B8887D0-9C0D-46DC-9D18-9F7354F8A351}" name="Description" dataDxfId="19">
+    <tableColumn id="8" xr3:uid="{2B8887D0-9C0D-46DC-9D18-9F7354F8A351}" name="Description" dataDxfId="11">
       <calculatedColumnFormula>"RARITY: " &amp; Table3[[#This Row],[Rarity]] &amp; " /// TIME: " &amp; Table3[[#This Row],[Time]] &amp; " /// LOCATION: " &amp; Table3[[#This Row],[Location]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5020,7 +4950,7 @@
     <tableColumn id="8" xr3:uid="{B87D96DA-876B-4321-974C-D3CA18927D46}" name="3-Heart Gifts"/>
     <tableColumn id="9" xr3:uid="{A8FFB3A6-3D98-46C6-9DA5-7615BB78E8C5}" name="2-Heart Gifts"/>
     <tableColumn id="10" xr3:uid="{2EF34846-880B-4FE1-BEBA-4EA7E502EABA}" name="1-Heart Gifts"/>
-    <tableColumn id="12" xr3:uid="{6D0FA26C-9E5B-468D-AD99-073C14547B04}" name="Description" dataDxfId="8">
+    <tableColumn id="12" xr3:uid="{6D0FA26C-9E5B-468D-AD99-073C14547B04}" name="Description" dataDxfId="10">
       <calculatedColumnFormula xml:space="preserve"> "Liked Gifts: " &amp; Table5[[#This Row],[Liked Gifts]] &amp; " /// 3-Heart Gifts: " &amp; Table5[[#This Row],[3-Heart Gifts]] &amp; " /// 2-Heart Gifts: " &amp; Table5[[#This Row],[2-Heart Gifts]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5347,8 +5277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B082B9-00AC-4E0F-A853-52691B39AEB7}">
   <dimension ref="A1:CJ62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BV1" workbookViewId="0">
-      <selection activeCell="CB10" sqref="CB10"/>
+    <sheetView tabSelected="1" topLeftCell="BQ1" workbookViewId="0">
+      <selection activeCell="BV3" sqref="BV3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5842,7 +5772,7 @@
         <v>1</v>
       </c>
       <c r="BQ2" s="2" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="BR2" s="2" t="s">
         <v>1103</v>
@@ -5853,16 +5783,16 @@
       <c r="BT2">
         <v>1</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="BU2" s="6" t="s">
         <v>1222</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="BV2" s="6" t="s">
         <v>909</v>
       </c>
       <c r="BW2">
         <v>3</v>
       </c>
-      <c r="BX2" s="3">
+      <c r="BX2" s="4">
         <v>1</v>
       </c>
       <c r="BY2" t="s">
@@ -5878,7 +5808,7 @@
         <v>204</v>
       </c>
       <c r="CD2" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="CE2">
         <v>1</v>
@@ -6071,19 +6001,22 @@
       <c r="BO3">
         <v>1</v>
       </c>
-      <c r="BQ3" t="s">
-        <v>1296</v>
-      </c>
-      <c r="BR3" t="s">
+      <c r="BQ3" s="2" t="s">
+        <v>1295</v>
+      </c>
+      <c r="BR3" s="2" t="s">
         <v>1110</v>
       </c>
       <c r="BS3">
         <v>1</v>
       </c>
-      <c r="BU3" t="s">
+      <c r="BT3">
+        <v>1</v>
+      </c>
+      <c r="BU3" s="6" t="s">
         <v>1226</v>
       </c>
-      <c r="BV3" t="s">
+      <c r="BV3" s="6" t="s">
         <v>913</v>
       </c>
       <c r="BW3">
@@ -6105,7 +6038,7 @@
         <v>211</v>
       </c>
       <c r="CD3" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="CE3">
         <v>1</v>
@@ -6296,7 +6229,7 @@
         <v>1</v>
       </c>
       <c r="BQ4" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="BR4" t="s">
         <v>1116</v>
@@ -6304,10 +6237,10 @@
       <c r="BS4">
         <v>1</v>
       </c>
-      <c r="BU4" t="s">
+      <c r="BU4" s="6" t="s">
         <v>1230</v>
       </c>
-      <c r="BV4" t="s">
+      <c r="BV4" s="6" t="s">
         <v>908</v>
       </c>
       <c r="BW4">
@@ -6329,7 +6262,7 @@
         <v>202</v>
       </c>
       <c r="CD4" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="CE4">
         <v>1</v>
@@ -6360,7 +6293,7 @@
       <c r="E5" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>104</v>
       </c>
       <c r="G5">
@@ -6382,7 +6315,7 @@
         <v>1</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>181</v>
@@ -6394,7 +6327,7 @@
         <v>1</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>179</v>
@@ -6451,7 +6384,7 @@
         <v>1</v>
       </c>
       <c r="AO5" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="AP5" t="s">
         <v>158</v>
@@ -6496,7 +6429,7 @@
         <v>1</v>
       </c>
       <c r="BI5" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="BJ5" t="s">
         <v>1154</v>
@@ -6514,7 +6447,7 @@
         <v>1</v>
       </c>
       <c r="BQ5" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="BR5" t="s">
         <v>1121</v>
@@ -6522,16 +6455,16 @@
       <c r="BS5">
         <v>1</v>
       </c>
-      <c r="BU5" t="s">
+      <c r="BU5" s="6" t="s">
         <v>1234</v>
       </c>
-      <c r="BV5" t="s">
+      <c r="BV5" s="6" t="s">
         <v>910</v>
       </c>
       <c r="BW5">
         <v>3</v>
       </c>
-      <c r="BX5" s="3">
+      <c r="BX5" s="4">
         <v>1</v>
       </c>
       <c r="BY5" t="s">
@@ -6547,7 +6480,7 @@
         <v>213</v>
       </c>
       <c r="CD5" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="CE5">
         <v>1</v>
@@ -6591,7 +6524,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>174</v>
@@ -6603,7 +6536,7 @@
         <v>1</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>175</v>
@@ -6615,7 +6548,7 @@
         <v>1</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>178</v>
@@ -6675,7 +6608,7 @@
         <v>1</v>
       </c>
       <c r="AO6" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="AP6" t="s">
         <v>159</v>
@@ -6723,7 +6656,7 @@
         <v>1</v>
       </c>
       <c r="BI6" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="BJ6" t="s">
         <v>1157</v>
@@ -6734,7 +6667,7 @@
       <c r="BM6" s="2" t="s">
         <v>1236</v>
       </c>
-      <c r="BN6" t="s">
+      <c r="BN6" s="2" t="s">
         <v>990</v>
       </c>
       <c r="BO6">
@@ -6744,7 +6677,7 @@
         <v>1</v>
       </c>
       <c r="BQ6" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="BR6" t="s">
         <v>1129</v>
@@ -6752,17 +6685,17 @@
       <c r="BS6">
         <v>1</v>
       </c>
-      <c r="BU6" t="s">
+      <c r="BU6" s="2" t="s">
         <v>1238</v>
       </c>
-      <c r="BV6" t="s">
+      <c r="BV6" s="2" t="s">
         <v>911</v>
       </c>
       <c r="BW6">
         <v>3</v>
       </c>
-      <c r="BX6" s="3">
-        <v>1</v>
+      <c r="BX6">
+        <v>3</v>
       </c>
       <c r="BY6" t="s">
         <v>615</v>
@@ -6777,7 +6710,7 @@
         <v>995</v>
       </c>
       <c r="CD6" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="CE6">
         <v>1</v>
@@ -6808,7 +6741,7 @@
       <c r="E7" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>108</v>
       </c>
       <c r="G7">
@@ -6818,7 +6751,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>175</v>
@@ -6830,7 +6763,7 @@
         <v>1</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>369</v>
@@ -6842,7 +6775,7 @@
         <v>1</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="R7" s="2" t="s">
         <v>180</v>
@@ -6899,7 +6832,7 @@
         <v>1</v>
       </c>
       <c r="AO7" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="AP7" t="s">
         <v>402</v>
@@ -6944,7 +6877,7 @@
         <v>1</v>
       </c>
       <c r="BI7" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="BJ7" t="s">
         <v>1158</v>
@@ -6953,9 +6886,9 @@
         <v>1</v>
       </c>
       <c r="BM7" s="2" t="s">
-        <v>1245</v>
-      </c>
-      <c r="BN7" t="s">
+        <v>1244</v>
+      </c>
+      <c r="BN7" s="2" t="s">
         <v>1218</v>
       </c>
       <c r="BO7">
@@ -6965,7 +6898,7 @@
         <v>1</v>
       </c>
       <c r="BQ7" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="BR7" t="s">
         <v>1130</v>
@@ -6973,17 +6906,17 @@
       <c r="BS7">
         <v>1</v>
       </c>
-      <c r="BU7" t="s">
+      <c r="BU7" s="6" t="s">
         <v>1241</v>
       </c>
-      <c r="BV7" t="s">
+      <c r="BV7" s="6" t="s">
         <v>912</v>
       </c>
       <c r="BW7">
         <v>3</v>
       </c>
       <c r="BX7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BY7" t="s">
         <v>618</v>
@@ -6998,7 +6931,7 @@
         <v>209</v>
       </c>
       <c r="CD7" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="CE7">
         <v>1</v>
@@ -7039,7 +6972,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>176</v>
@@ -7051,7 +6984,7 @@
         <v>1</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>370</v>
@@ -7084,7 +7017,7 @@
         <v>1</v>
       </c>
       <c r="Y8" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="Z8" t="s">
         <v>304</v>
@@ -7093,7 +7026,7 @@
         <v>1</v>
       </c>
       <c r="AC8" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="AD8" t="s">
         <v>418</v>
@@ -7120,7 +7053,7 @@
         <v>1</v>
       </c>
       <c r="AO8" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="AP8" t="s">
         <v>164</v>
@@ -7165,7 +7098,7 @@
         <v>1</v>
       </c>
       <c r="BI8" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="BJ8" t="s">
         <v>1159</v>
@@ -7173,17 +7106,20 @@
       <c r="BK8">
         <v>1</v>
       </c>
-      <c r="BM8" t="s">
-        <v>1246</v>
-      </c>
-      <c r="BN8" t="s">
+      <c r="BM8" s="2" t="s">
+        <v>1245</v>
+      </c>
+      <c r="BN8" s="2" t="s">
         <v>990</v>
       </c>
       <c r="BO8">
         <v>1</v>
       </c>
+      <c r="BP8">
+        <v>1</v>
+      </c>
       <c r="BQ8" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="BR8" t="s">
         <v>1131</v>
@@ -7191,17 +7127,17 @@
       <c r="BS8">
         <v>1</v>
       </c>
-      <c r="BU8" t="s">
-        <v>1244</v>
-      </c>
-      <c r="BV8" t="s">
+      <c r="BU8" s="6" t="s">
+        <v>1532</v>
+      </c>
+      <c r="BV8" s="6" t="s">
         <v>815</v>
       </c>
       <c r="BW8">
         <v>3</v>
       </c>
-      <c r="BX8" s="3">
-        <v>1</v>
+      <c r="BX8">
+        <v>2</v>
       </c>
       <c r="BY8" t="s">
         <v>621</v>
@@ -7216,7 +7152,7 @@
         <v>205</v>
       </c>
       <c r="CD8" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="CE8">
         <v>1</v>
@@ -7275,7 +7211,7 @@
         <v>1</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>158</v>
@@ -7296,7 +7232,7 @@
         <v>1</v>
       </c>
       <c r="Y9" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="Z9" t="s">
         <v>305</v>
@@ -7305,7 +7241,7 @@
         <v>1</v>
       </c>
       <c r="AC9" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="AD9" t="s">
         <v>419</v>
@@ -7332,7 +7268,7 @@
         <v>1</v>
       </c>
       <c r="AO9" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="AP9" t="s">
         <v>162</v>
@@ -7368,7 +7304,7 @@
         <v>1</v>
       </c>
       <c r="BI9" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="BJ9" t="s">
         <v>1160</v>
@@ -7377,9 +7313,9 @@
         <v>1</v>
       </c>
       <c r="BM9" s="2" t="s">
-        <v>1248</v>
-      </c>
-      <c r="BN9" t="s">
+        <v>1247</v>
+      </c>
+      <c r="BN9" s="2" t="s">
         <v>1218</v>
       </c>
       <c r="BO9">
@@ -7389,7 +7325,7 @@
         <v>1</v>
       </c>
       <c r="BQ9" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="BR9" t="s">
         <v>1132</v>
@@ -7397,17 +7333,17 @@
       <c r="BS9">
         <v>1</v>
       </c>
-      <c r="BU9" t="s">
-        <v>1250</v>
-      </c>
-      <c r="BV9" t="s">
+      <c r="BU9" s="6" t="s">
+        <v>1249</v>
+      </c>
+      <c r="BV9" s="6" t="s">
         <v>920</v>
       </c>
       <c r="BW9">
         <v>3</v>
       </c>
       <c r="BX9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BY9" t="s">
         <v>624</v>
@@ -7422,7 +7358,7 @@
         <v>206</v>
       </c>
       <c r="CD9" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="CE9">
         <v>1</v>
@@ -7453,7 +7389,7 @@
       <c r="E10" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>116</v>
       </c>
       <c r="G10">
@@ -7484,7 +7420,7 @@
         <v>1</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="R10" s="2" t="s">
         <v>159</v>
@@ -7496,7 +7432,7 @@
         <v>1</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="V10" s="2" t="s">
         <v>176</v>
@@ -7517,7 +7453,7 @@
         <v>1</v>
       </c>
       <c r="AC10" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="AD10" t="s">
         <v>420</v>
@@ -7544,7 +7480,7 @@
         <v>1</v>
       </c>
       <c r="AO10" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="AP10" t="s">
         <v>175</v>
@@ -7580,7 +7516,7 @@
         <v>1</v>
       </c>
       <c r="BI10" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="BJ10" t="s">
         <v>1161</v>
@@ -7589,9 +7525,9 @@
         <v>1</v>
       </c>
       <c r="BM10" s="2" t="s">
-        <v>1252</v>
-      </c>
-      <c r="BN10" t="s">
+        <v>1251</v>
+      </c>
+      <c r="BN10" s="2" t="s">
         <v>990</v>
       </c>
       <c r="BO10">
@@ -7601,7 +7537,7 @@
         <v>1</v>
       </c>
       <c r="BQ10" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="BR10" t="s">
         <v>1133</v>
@@ -7609,17 +7545,17 @@
       <c r="BS10">
         <v>1</v>
       </c>
-      <c r="BU10" t="s">
-        <v>1254</v>
-      </c>
-      <c r="BV10" t="s">
+      <c r="BU10" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="BV10" s="2" t="s">
         <v>917</v>
       </c>
       <c r="BW10">
         <v>3</v>
       </c>
       <c r="BX10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BY10" t="s">
         <v>627</v>
@@ -7634,7 +7570,7 @@
         <v>216</v>
       </c>
       <c r="CD10" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="CE10">
         <v>1</v>
@@ -7653,7 +7589,7 @@
       <c r="E11" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>114</v>
       </c>
       <c r="G11">
@@ -7687,7 +7623,7 @@
         <v>1</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="R11" s="2" t="s">
         <v>164</v>
@@ -7699,7 +7635,7 @@
         <v>1</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="V11" s="2" t="s">
         <v>175</v>
@@ -7723,7 +7659,7 @@
         <v>1</v>
       </c>
       <c r="AC11" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="AD11" t="s">
         <v>421</v>
@@ -7750,7 +7686,7 @@
         <v>1</v>
       </c>
       <c r="AO11" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="AP11" t="s">
         <v>176</v>
@@ -7786,7 +7722,7 @@
         <v>1</v>
       </c>
       <c r="BI11" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="BJ11" t="s">
         <v>1162</v>
@@ -7795,9 +7731,9 @@
         <v>1</v>
       </c>
       <c r="BM11" s="2" t="s">
-        <v>1256</v>
-      </c>
-      <c r="BN11" t="s">
+        <v>1255</v>
+      </c>
+      <c r="BN11" s="2" t="s">
         <v>1218</v>
       </c>
       <c r="BO11">
@@ -7807,7 +7743,7 @@
         <v>1</v>
       </c>
       <c r="BQ11" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="BR11" t="s">
         <v>1137</v>
@@ -7815,16 +7751,16 @@
       <c r="BS11">
         <v>1</v>
       </c>
-      <c r="BU11" t="s">
-        <v>1258</v>
-      </c>
-      <c r="BV11" t="s">
+      <c r="BU11" s="6" t="s">
+        <v>1257</v>
+      </c>
+      <c r="BV11" s="6" t="s">
         <v>914</v>
       </c>
       <c r="BW11">
         <v>3</v>
       </c>
-      <c r="BX11" s="3">
+      <c r="BX11" s="4">
         <v>1</v>
       </c>
       <c r="BY11" t="s">
@@ -7840,7 +7776,7 @@
         <v>207</v>
       </c>
       <c r="CD11" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="CE11">
         <v>1</v>
@@ -7856,13 +7792,16 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>118</v>
       </c>
       <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
         <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
@@ -7887,7 +7826,7 @@
         <v>1</v>
       </c>
       <c r="Q12" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="R12" t="s">
         <v>402</v>
@@ -7914,7 +7853,7 @@
         <v>1</v>
       </c>
       <c r="AC12" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="AD12" t="s">
         <v>422</v>
@@ -7941,7 +7880,7 @@
         <v>1</v>
       </c>
       <c r="AO12" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="AP12" t="s">
         <v>180</v>
@@ -7977,7 +7916,7 @@
         <v>1</v>
       </c>
       <c r="BI12" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="BJ12" t="s">
         <v>1164</v>
@@ -7986,9 +7925,9 @@
         <v>1</v>
       </c>
       <c r="BM12" s="2" t="s">
-        <v>1260</v>
-      </c>
-      <c r="BN12" t="s">
+        <v>1259</v>
+      </c>
+      <c r="BN12" s="2" t="s">
         <v>990</v>
       </c>
       <c r="BO12">
@@ -7998,7 +7937,7 @@
         <v>1</v>
       </c>
       <c r="BQ12" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="BR12" t="s">
         <v>1138</v>
@@ -8006,10 +7945,10 @@
       <c r="BS12">
         <v>1</v>
       </c>
-      <c r="BU12" t="s">
-        <v>1262</v>
-      </c>
-      <c r="BV12" t="s">
+      <c r="BU12" s="6" t="s">
+        <v>1261</v>
+      </c>
+      <c r="BV12" s="6" t="s">
         <v>916</v>
       </c>
       <c r="BW12">
@@ -8031,7 +7970,7 @@
         <v>210</v>
       </c>
       <c r="CD12" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="CE12">
         <v>1</v>
@@ -8047,13 +7986,16 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
         <v>1</v>
       </c>
       <c r="I13" t="s">
@@ -8138,7 +8080,7 @@
         <v>1</v>
       </c>
       <c r="AO13" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="AP13" t="s">
         <v>178</v>
@@ -8174,7 +8116,7 @@
         <v>1</v>
       </c>
       <c r="BI13" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="BJ13" t="s">
         <v>1166</v>
@@ -8182,17 +8124,20 @@
       <c r="BK13">
         <v>1</v>
       </c>
-      <c r="BM13" t="s">
-        <v>1303</v>
-      </c>
-      <c r="BN13" t="s">
+      <c r="BM13" s="2" t="s">
+        <v>1302</v>
+      </c>
+      <c r="BN13" s="2" t="s">
         <v>991</v>
       </c>
       <c r="BO13">
         <v>1</v>
       </c>
+      <c r="BP13">
+        <v>1</v>
+      </c>
       <c r="BQ13" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="BR13" t="s">
         <v>1134</v>
@@ -8200,16 +8145,16 @@
       <c r="BS13">
         <v>1</v>
       </c>
-      <c r="BU13" t="s">
-        <v>1265</v>
-      </c>
-      <c r="BV13" t="s">
+      <c r="BU13" s="6" t="s">
+        <v>1264</v>
+      </c>
+      <c r="BV13" s="6" t="s">
         <v>918</v>
       </c>
       <c r="BW13">
         <v>3</v>
       </c>
-      <c r="BX13" s="3">
+      <c r="BX13" s="4">
         <v>1</v>
       </c>
       <c r="BY13" t="s">
@@ -8225,7 +8170,7 @@
         <v>212</v>
       </c>
       <c r="CD13" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="CE13">
         <v>1</v>
@@ -8244,7 +8189,7 @@
       <c r="E14" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>124</v>
       </c>
       <c r="G14">
@@ -8371,7 +8316,7 @@
         <v>1</v>
       </c>
       <c r="BI14" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="BJ14" t="s">
         <v>1167</v>
@@ -8380,9 +8325,9 @@
         <v>1</v>
       </c>
       <c r="BM14" s="2" t="s">
-        <v>1304</v>
-      </c>
-      <c r="BN14" t="s">
+        <v>1303</v>
+      </c>
+      <c r="BN14" s="2" t="s">
         <v>992</v>
       </c>
       <c r="BO14">
@@ -8392,7 +8337,7 @@
         <v>1</v>
       </c>
       <c r="BQ14" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="BR14" t="s">
         <v>1135</v>
@@ -8400,17 +8345,17 @@
       <c r="BS14">
         <v>1</v>
       </c>
-      <c r="BU14" t="s">
-        <v>1268</v>
-      </c>
-      <c r="BV14" t="s">
+      <c r="BU14" s="2" t="s">
+        <v>1267</v>
+      </c>
+      <c r="BV14" s="2" t="s">
         <v>915</v>
       </c>
       <c r="BW14">
         <v>3</v>
       </c>
-      <c r="BX14" s="3">
-        <v>2</v>
+      <c r="BX14">
+        <v>3</v>
       </c>
       <c r="BY14" t="s">
         <v>641</v>
@@ -8425,7 +8370,7 @@
         <v>203</v>
       </c>
       <c r="CD14" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="CE14">
         <v>1</v>
@@ -8444,7 +8389,7 @@
       <c r="E15" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>122</v>
       </c>
       <c r="G15">
@@ -8475,7 +8420,7 @@
         <v>1</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="R15" s="2" t="s">
         <v>175</v>
@@ -8487,7 +8432,7 @@
         <v>1</v>
       </c>
       <c r="U15" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="V15" t="s">
         <v>218</v>
@@ -8571,7 +8516,7 @@
         <v>1</v>
       </c>
       <c r="BI15" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="BJ15" t="s">
         <v>1168</v>
@@ -8579,17 +8524,20 @@
       <c r="BK15">
         <v>1</v>
       </c>
-      <c r="BM15" t="s">
-        <v>1305</v>
-      </c>
-      <c r="BN15" t="s">
+      <c r="BM15" s="2" t="s">
+        <v>1304</v>
+      </c>
+      <c r="BN15" s="2" t="s">
         <v>992</v>
       </c>
       <c r="BO15">
         <v>1</v>
       </c>
+      <c r="BP15">
+        <v>1</v>
+      </c>
       <c r="BQ15" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="BR15" t="s">
         <v>1136</v>
@@ -8597,10 +8545,10 @@
       <c r="BS15">
         <v>1</v>
       </c>
-      <c r="BU15" t="s">
-        <v>1270</v>
-      </c>
-      <c r="BV15" t="s">
+      <c r="BU15" s="6" t="s">
+        <v>1269</v>
+      </c>
+      <c r="BV15" s="6" t="s">
         <v>919</v>
       </c>
       <c r="BW15">
@@ -8622,7 +8570,7 @@
         <v>214</v>
       </c>
       <c r="CD15" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="CE15">
         <v>1</v>
@@ -8651,7 +8599,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>173</v>
@@ -8675,7 +8623,7 @@
         <v>1</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="R16" s="2" t="s">
         <v>176</v>
@@ -8687,7 +8635,7 @@
         <v>1</v>
       </c>
       <c r="U16" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="V16" t="s">
         <v>219</v>
@@ -8705,7 +8653,7 @@
         <v>1</v>
       </c>
       <c r="AC16" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="AD16" t="s">
         <v>424</v>
@@ -8759,7 +8707,7 @@
         <v>1</v>
       </c>
       <c r="BI16" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="BJ16" t="s">
         <v>1169</v>
@@ -8767,17 +8715,20 @@
       <c r="BK16">
         <v>1</v>
       </c>
-      <c r="BM16" t="s">
-        <v>1306</v>
-      </c>
-      <c r="BN16" t="s">
+      <c r="BM16" s="2" t="s">
+        <v>1305</v>
+      </c>
+      <c r="BN16" s="2" t="s">
         <v>1218</v>
       </c>
       <c r="BO16">
         <v>1</v>
       </c>
+      <c r="BP16">
+        <v>1</v>
+      </c>
       <c r="BQ16" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="BR16" t="s">
         <v>1139</v>
@@ -8786,7 +8737,7 @@
         <v>1</v>
       </c>
       <c r="BU16" s="2" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="BV16" s="2" t="s">
         <v>923</v>
@@ -8810,7 +8761,7 @@
         <v>215</v>
       </c>
       <c r="CD16" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="CE16">
         <v>1</v>
@@ -8836,7 +8787,7 @@
         <v>1</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>177</v>
@@ -8866,7 +8817,7 @@
         <v>1</v>
       </c>
       <c r="U17" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="V17" t="s">
         <v>220</v>
@@ -8887,7 +8838,7 @@
         <v>1</v>
       </c>
       <c r="AC17" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="AD17" t="s">
         <v>425</v>
@@ -8941,7 +8892,7 @@
         <v>1</v>
       </c>
       <c r="BI17" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="BJ17" t="s">
         <v>1170</v>
@@ -8950,7 +8901,7 @@
         <v>1</v>
       </c>
       <c r="BM17" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="BN17" t="s">
         <v>993</v>
@@ -8959,7 +8910,7 @@
         <v>1</v>
       </c>
       <c r="BQ17" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="BR17" t="s">
         <v>987</v>
@@ -8968,7 +8919,7 @@
         <v>1</v>
       </c>
       <c r="BU17" s="2" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="BV17" s="2" t="s">
         <v>922</v>
@@ -8992,7 +8943,7 @@
         <v>1009</v>
       </c>
       <c r="CD17" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="CE17">
         <v>1</v>
@@ -9021,7 +8972,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>179</v>
@@ -9054,7 +9005,7 @@
         <v>1</v>
       </c>
       <c r="U18" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="V18" t="s">
         <v>221</v>
@@ -9072,7 +9023,7 @@
         <v>1</v>
       </c>
       <c r="AC18" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="AD18" t="s">
         <v>426</v>
@@ -9126,7 +9077,7 @@
         <v>1</v>
       </c>
       <c r="BI18" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="BJ18" t="s">
         <v>1171</v>
@@ -9134,17 +9085,20 @@
       <c r="BK18">
         <v>1</v>
       </c>
-      <c r="BM18" t="s">
-        <v>1308</v>
-      </c>
-      <c r="BN18" t="s">
+      <c r="BM18" s="2" t="s">
+        <v>1307</v>
+      </c>
+      <c r="BN18" s="2" t="s">
         <v>1218</v>
       </c>
       <c r="BO18">
         <v>1</v>
       </c>
+      <c r="BP18">
+        <v>1</v>
+      </c>
       <c r="BQ18" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="BR18" t="s">
         <v>1139</v>
@@ -9153,7 +9107,7 @@
         <v>1</v>
       </c>
       <c r="BU18" s="2" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="BV18" s="2" t="s">
         <v>845</v>
@@ -9177,7 +9131,7 @@
         <v>1010</v>
       </c>
       <c r="CD18" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="CE18">
         <v>1</v>
@@ -9203,7 +9157,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>178</v>
@@ -9236,7 +9190,7 @@
         <v>1</v>
       </c>
       <c r="U19" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="V19" t="s">
         <v>222</v>
@@ -9254,7 +9208,7 @@
         <v>1</v>
       </c>
       <c r="AC19" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="AD19" t="s">
         <v>427</v>
@@ -9299,7 +9253,7 @@
         <v>1</v>
       </c>
       <c r="BI19" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="BJ19" t="s">
         <v>1172</v>
@@ -9307,17 +9261,20 @@
       <c r="BK19">
         <v>1</v>
       </c>
-      <c r="BM19" t="s">
-        <v>1309</v>
-      </c>
-      <c r="BN19" t="s">
+      <c r="BM19" s="2" t="s">
+        <v>1308</v>
+      </c>
+      <c r="BN19" s="2" t="s">
         <v>992</v>
       </c>
       <c r="BO19">
         <v>1</v>
       </c>
+      <c r="BP19">
+        <v>1</v>
+      </c>
       <c r="BQ19" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="BR19" t="s">
         <v>987</v>
@@ -9326,7 +9283,7 @@
         <v>1</v>
       </c>
       <c r="BU19" s="2" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="BV19" s="2" t="s">
         <v>924</v>
@@ -9350,7 +9307,7 @@
         <v>1011</v>
       </c>
       <c r="CD19" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="CE19">
         <v>1</v>
@@ -9376,7 +9333,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>180</v>
@@ -9412,7 +9369,7 @@
         <v>1</v>
       </c>
       <c r="U20" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="V20" t="s">
         <v>233</v>
@@ -9430,7 +9387,7 @@
         <v>1</v>
       </c>
       <c r="AC20" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="AD20" t="s">
         <v>428</v>
@@ -9475,7 +9432,7 @@
         <v>1</v>
       </c>
       <c r="BI20" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="BJ20" t="s">
         <v>1173</v>
@@ -9483,17 +9440,20 @@
       <c r="BK20">
         <v>1</v>
       </c>
-      <c r="BM20" t="s">
-        <v>1310</v>
-      </c>
-      <c r="BN20" t="s">
+      <c r="BM20" s="2" t="s">
+        <v>1309</v>
+      </c>
+      <c r="BN20" s="2" t="s">
         <v>992</v>
       </c>
       <c r="BO20">
         <v>1</v>
       </c>
+      <c r="BP20">
+        <v>1</v>
+      </c>
       <c r="BQ20" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="BR20" t="s">
         <v>1140</v>
@@ -9502,7 +9462,7 @@
         <v>1</v>
       </c>
       <c r="BU20" s="2" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="BV20" s="2" t="s">
         <v>925</v>
@@ -9526,7 +9486,7 @@
         <v>1012</v>
       </c>
       <c r="CD20" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="CE20">
         <v>1</v>
@@ -9548,7 +9508,7 @@
       <c r="E21" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="2" t="s">
         <v>1217</v>
       </c>
       <c r="G21">
@@ -9558,7 +9518,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>165</v>
@@ -9588,7 +9548,7 @@
         <v>1</v>
       </c>
       <c r="U21" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="V21" t="s">
         <v>234</v>
@@ -9609,7 +9569,7 @@
         <v>1</v>
       </c>
       <c r="AC21" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="AD21" t="s">
         <v>429</v>
@@ -9645,7 +9605,7 @@
         <v>1</v>
       </c>
       <c r="BI21" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="BJ21" t="s">
         <v>1175</v>
@@ -9654,9 +9614,9 @@
         <v>1</v>
       </c>
       <c r="BM21" s="2" t="s">
-        <v>1288</v>
-      </c>
-      <c r="BN21" t="s">
+        <v>1287</v>
+      </c>
+      <c r="BN21" s="2" t="s">
         <v>991</v>
       </c>
       <c r="BO21">
@@ -9666,7 +9626,7 @@
         <v>1</v>
       </c>
       <c r="BQ21" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="BR21" t="s">
         <v>1141</v>
@@ -9675,7 +9635,7 @@
         <v>1</v>
       </c>
       <c r="BU21" s="2" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="BV21" s="2" t="s">
         <v>921</v>
@@ -9699,7 +9659,7 @@
         <v>1013</v>
       </c>
       <c r="CD21" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="CE21">
         <v>1</v>
@@ -9737,7 +9697,7 @@
         <v>1</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>179</v>
@@ -9749,7 +9709,7 @@
         <v>1</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="R22" s="2" t="s">
         <v>173</v>
@@ -9761,7 +9721,7 @@
         <v>1</v>
       </c>
       <c r="U22" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="V22" t="s">
         <v>235</v>
@@ -9782,7 +9742,7 @@
         <v>1</v>
       </c>
       <c r="AC22" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="AD22" t="s">
         <v>430</v>
@@ -9818,7 +9778,7 @@
         <v>1</v>
       </c>
       <c r="BI22" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="BJ22" t="s">
         <v>1176</v>
@@ -9827,7 +9787,7 @@
         <v>1</v>
       </c>
       <c r="BM22" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="BN22" t="s">
         <v>992</v>
@@ -9836,7 +9796,7 @@
         <v>1</v>
       </c>
       <c r="BQ22" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="BR22" t="s">
         <v>988</v>
@@ -9844,10 +9804,10 @@
       <c r="BS22">
         <v>1</v>
       </c>
-      <c r="BU22" t="s">
-        <v>1311</v>
-      </c>
-      <c r="BV22" t="s">
+      <c r="BU22" s="6" t="s">
+        <v>1310</v>
+      </c>
+      <c r="BV22" s="6" t="s">
         <v>927</v>
       </c>
       <c r="BW22">
@@ -9886,7 +9846,7 @@
         <v>1</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>178</v>
@@ -9898,7 +9858,7 @@
         <v>1</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="R23" s="2" t="s">
         <v>177</v>
@@ -9910,7 +9870,7 @@
         <v>1</v>
       </c>
       <c r="U23" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="V23" t="s">
         <v>236</v>
@@ -9930,16 +9890,18 @@
       <c r="AB23">
         <v>1</v>
       </c>
-      <c r="AC23" t="s">
-        <v>1502</v>
-      </c>
-      <c r="AD23" t="s">
+      <c r="AC23" s="2" t="s">
+        <v>1501</v>
+      </c>
+      <c r="AD23" s="2" t="s">
         <v>177</v>
       </c>
       <c r="AE23">
         <v>1</v>
       </c>
-      <c r="AF23" s="2"/>
+      <c r="AF23">
+        <v>1</v>
+      </c>
       <c r="AS23" t="s">
         <v>553</v>
       </c>
@@ -9950,7 +9912,7 @@
         <v>1</v>
       </c>
       <c r="BI23" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="BJ23" t="s">
         <v>1177</v>
@@ -9959,9 +9921,9 @@
         <v>1</v>
       </c>
       <c r="BM23" s="2" t="s">
-        <v>1295</v>
-      </c>
-      <c r="BN23" t="s">
+        <v>1294</v>
+      </c>
+      <c r="BN23" s="2" t="s">
         <v>1218</v>
       </c>
       <c r="BO23">
@@ -9971,7 +9933,7 @@
         <v>1</v>
       </c>
       <c r="BQ23" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="BR23" t="s">
         <v>1142</v>
@@ -9979,10 +9941,10 @@
       <c r="BS23">
         <v>1</v>
       </c>
-      <c r="BU23" t="s">
-        <v>1312</v>
-      </c>
-      <c r="BV23" t="s">
+      <c r="BU23" s="6" t="s">
+        <v>1311</v>
+      </c>
+      <c r="BV23" s="6" t="s">
         <v>930</v>
       </c>
       <c r="BW23">
@@ -10024,7 +9986,7 @@
         <v>1</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="N24" s="2" t="s">
         <v>180</v>
@@ -10036,7 +9998,7 @@
         <v>1</v>
       </c>
       <c r="Q24" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="R24" t="s">
         <v>387</v>
@@ -10065,18 +10027,20 @@
       <c r="AA24">
         <v>1</v>
       </c>
-      <c r="AC24" t="s">
-        <v>1503</v>
-      </c>
-      <c r="AD24" t="s">
+      <c r="AC24" s="2" t="s">
+        <v>1502</v>
+      </c>
+      <c r="AD24" s="2" t="s">
         <v>173</v>
       </c>
       <c r="AE24">
         <v>1</v>
       </c>
-      <c r="AF24" s="2"/>
+      <c r="AF24">
+        <v>1</v>
+      </c>
       <c r="BI24" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="BJ24" t="s">
         <v>1180</v>
@@ -10085,7 +10049,7 @@
         <v>1</v>
       </c>
       <c r="BM24" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="BN24" t="s">
         <v>993</v>
@@ -10094,7 +10058,7 @@
         <v>1</v>
       </c>
       <c r="BQ24" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="BR24" t="s">
         <v>989</v>
@@ -10102,16 +10066,16 @@
       <c r="BS24">
         <v>1</v>
       </c>
-      <c r="BU24" t="s">
-        <v>1314</v>
-      </c>
-      <c r="BV24" t="s">
+      <c r="BU24" s="6" t="s">
+        <v>1313</v>
+      </c>
+      <c r="BV24" s="6" t="s">
         <v>934</v>
       </c>
       <c r="BW24">
         <v>3</v>
       </c>
-      <c r="BX24" s="3">
+      <c r="BX24" s="4">
         <v>1</v>
       </c>
     </row>
@@ -10128,7 +10092,7 @@
       <c r="E25" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="2" t="s">
         <v>141</v>
       </c>
       <c r="G25">
@@ -10150,7 +10114,7 @@
         <v>1</v>
       </c>
       <c r="Q25" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="R25" t="s">
         <v>388</v>
@@ -10189,7 +10153,7 @@
         <v>1</v>
       </c>
       <c r="BI25" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="BJ25" t="s">
         <v>1181</v>
@@ -10198,9 +10162,9 @@
         <v>1</v>
       </c>
       <c r="BM25" s="2" t="s">
-        <v>1300</v>
-      </c>
-      <c r="BN25" t="s">
+        <v>1299</v>
+      </c>
+      <c r="BN25" s="2" t="s">
         <v>990</v>
       </c>
       <c r="BO25">
@@ -10210,7 +10174,7 @@
         <v>1</v>
       </c>
       <c r="BQ25" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="BR25" t="s">
         <v>1143</v>
@@ -10218,16 +10182,16 @@
       <c r="BS25">
         <v>1</v>
       </c>
-      <c r="BU25" t="s">
-        <v>1316</v>
-      </c>
-      <c r="BV25" t="s">
+      <c r="BU25" s="6" t="s">
+        <v>1315</v>
+      </c>
+      <c r="BV25" s="6" t="s">
         <v>932</v>
       </c>
       <c r="BW25">
         <v>3</v>
       </c>
-      <c r="BX25" s="3">
+      <c r="BX25" s="4">
         <v>1</v>
       </c>
     </row>
@@ -10260,7 +10224,7 @@
         <v>1</v>
       </c>
       <c r="Q26" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="R26" t="s">
         <v>390</v>
@@ -10290,7 +10254,7 @@
         <v>1</v>
       </c>
       <c r="BI26" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="BJ26" t="s">
         <v>1186</v>
@@ -10299,7 +10263,7 @@
         <v>1</v>
       </c>
       <c r="BM26" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="BN26" t="s">
         <v>1218</v>
@@ -10308,7 +10272,7 @@
         <v>1</v>
       </c>
       <c r="BQ26" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="BR26" t="s">
         <v>985</v>
@@ -10316,16 +10280,16 @@
       <c r="BS26">
         <v>1</v>
       </c>
-      <c r="BU26" t="s">
-        <v>1318</v>
-      </c>
-      <c r="BV26" t="s">
+      <c r="BU26" s="6" t="s">
+        <v>1317</v>
+      </c>
+      <c r="BV26" s="6" t="s">
         <v>928</v>
       </c>
       <c r="BW26">
         <v>3</v>
       </c>
-      <c r="BX26" s="3">
+      <c r="BX26" s="4">
         <v>1</v>
       </c>
     </row>
@@ -10379,7 +10343,7 @@
         <v>1</v>
       </c>
       <c r="BI27" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="BJ27" t="s">
         <v>1187</v>
@@ -10388,7 +10352,7 @@
         <v>1</v>
       </c>
       <c r="BM27" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="BN27" t="s">
         <v>1218</v>
@@ -10408,16 +10372,16 @@
       <c r="BT27">
         <v>1</v>
       </c>
-      <c r="BU27" t="s">
-        <v>1320</v>
-      </c>
-      <c r="BV27" t="s">
+      <c r="BU27" s="6" t="s">
+        <v>1319</v>
+      </c>
+      <c r="BV27" s="6" t="s">
         <v>933</v>
       </c>
       <c r="BW27">
         <v>3</v>
       </c>
-      <c r="BX27" s="3">
+      <c r="BX27" s="4">
         <v>1</v>
       </c>
     </row>
@@ -10468,7 +10432,7 @@
         <v>1</v>
       </c>
       <c r="BI28" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="BJ28" t="s">
         <v>1188</v>
@@ -10477,7 +10441,7 @@
         <v>1</v>
       </c>
       <c r="BM28" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="BN28" t="s">
         <v>1218</v>
@@ -10497,17 +10461,17 @@
       <c r="BT28">
         <v>1</v>
       </c>
-      <c r="BU28" t="s">
-        <v>1323</v>
-      </c>
-      <c r="BV28" t="s">
+      <c r="BU28" s="6" t="s">
+        <v>1322</v>
+      </c>
+      <c r="BV28" s="6" t="s">
         <v>929</v>
       </c>
       <c r="BW28">
         <v>3</v>
       </c>
       <c r="BX28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:83" x14ac:dyDescent="0.25">
@@ -10551,7 +10515,7 @@
         <v>1</v>
       </c>
       <c r="BI29" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="BJ29" t="s">
         <v>1189</v>
@@ -10560,7 +10524,7 @@
         <v>1</v>
       </c>
       <c r="BM29" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="BN29" t="s">
         <v>1218</v>
@@ -10580,17 +10544,17 @@
       <c r="BT29">
         <v>1</v>
       </c>
-      <c r="BU29" t="s">
-        <v>1326</v>
-      </c>
-      <c r="BV29" t="s">
+      <c r="BU29" s="6" t="s">
+        <v>1325</v>
+      </c>
+      <c r="BV29" s="6" t="s">
         <v>926</v>
       </c>
       <c r="BW29">
         <v>3</v>
       </c>
       <c r="BX29">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:83" x14ac:dyDescent="0.25">
@@ -10622,7 +10586,7 @@
         <v>1</v>
       </c>
       <c r="Y30" s="2" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="Z30" s="2" t="s">
         <v>178</v>
@@ -10634,7 +10598,7 @@
         <v>1</v>
       </c>
       <c r="BI30" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="BJ30" t="s">
         <v>1190</v>
@@ -10643,7 +10607,7 @@
         <v>1</v>
       </c>
       <c r="BM30" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="BN30" t="s">
         <v>1218</v>
@@ -10663,17 +10627,17 @@
       <c r="BT30">
         <v>1</v>
       </c>
-      <c r="BU30" t="s">
-        <v>1329</v>
-      </c>
-      <c r="BV30" t="s">
+      <c r="BU30" s="6" t="s">
+        <v>1328</v>
+      </c>
+      <c r="BV30" s="6" t="s">
         <v>931</v>
       </c>
       <c r="BW30">
         <v>3</v>
       </c>
-      <c r="BX30" s="3">
-        <v>1</v>
+      <c r="BX30">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:83" x14ac:dyDescent="0.25">
@@ -10705,7 +10669,7 @@
         <v>1</v>
       </c>
       <c r="Y31" s="2" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="Z31" s="2" t="s">
         <v>254</v>
@@ -10717,7 +10681,7 @@
         <v>1</v>
       </c>
       <c r="BI31" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="BJ31" t="s">
         <v>1191</v>
@@ -10726,9 +10690,9 @@
         <v>1</v>
       </c>
       <c r="BM31" s="2" t="s">
-        <v>1358</v>
-      </c>
-      <c r="BN31" t="s">
+        <v>1357</v>
+      </c>
+      <c r="BN31" s="2" t="s">
         <v>1218</v>
       </c>
       <c r="BO31">
@@ -10749,16 +10713,16 @@
       <c r="BT31">
         <v>1</v>
       </c>
-      <c r="BU31" t="s">
-        <v>1332</v>
-      </c>
-      <c r="BV31" t="s">
+      <c r="BU31" s="6" t="s">
+        <v>1331</v>
+      </c>
+      <c r="BV31" s="6" t="s">
         <v>935</v>
       </c>
       <c r="BW31">
         <v>3</v>
       </c>
-      <c r="BX31" s="3">
+      <c r="BX31" s="4">
         <v>1</v>
       </c>
     </row>
@@ -10791,7 +10755,7 @@
         <v>1</v>
       </c>
       <c r="Y32" s="2" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="Z32" s="2" t="s">
         <v>179</v>
@@ -10803,7 +10767,7 @@
         <v>1</v>
       </c>
       <c r="BI32" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="BJ32" t="s">
         <v>1192</v>
@@ -10812,7 +10776,7 @@
         <v>1</v>
       </c>
       <c r="BM32" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="BN32" t="s">
         <v>1218</v>
@@ -10833,7 +10797,7 @@
         <v>1</v>
       </c>
       <c r="BU32" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="BV32" t="s">
         <v>936</v>
@@ -10883,7 +10847,7 @@
         <v>1</v>
       </c>
       <c r="BI33" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="BJ33" t="s">
         <v>1182</v>
@@ -10892,7 +10856,7 @@
         <v>1</v>
       </c>
       <c r="BM33" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="BN33" t="s">
         <v>992</v>
@@ -10912,10 +10876,10 @@
       <c r="BT33">
         <v>1</v>
       </c>
-      <c r="BU33" t="s">
-        <v>1338</v>
-      </c>
-      <c r="BV33" t="s">
+      <c r="BU33" s="6" t="s">
+        <v>1337</v>
+      </c>
+      <c r="BV33" s="6" t="s">
         <v>938</v>
       </c>
       <c r="BW33">
@@ -10939,7 +10903,7 @@
         <v>1</v>
       </c>
       <c r="U34" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="V34" t="s">
         <v>241</v>
@@ -10957,7 +10921,7 @@
         <v>1</v>
       </c>
       <c r="BI34" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="BJ34" t="s">
         <v>1183</v>
@@ -10966,7 +10930,7 @@
         <v>1</v>
       </c>
       <c r="BM34" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="BN34" t="s">
         <v>1218</v>
@@ -10975,7 +10939,7 @@
         <v>1</v>
       </c>
       <c r="BQ34" s="2" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="BR34" s="2" t="s">
         <v>1098</v>
@@ -10986,16 +10950,16 @@
       <c r="BT34">
         <v>1</v>
       </c>
-      <c r="BU34" t="s">
-        <v>1341</v>
-      </c>
-      <c r="BV34" t="s">
+      <c r="BU34" s="6" t="s">
+        <v>1340</v>
+      </c>
+      <c r="BV34" s="6" t="s">
         <v>937</v>
       </c>
       <c r="BW34">
         <v>3</v>
       </c>
-      <c r="BX34" s="3">
+      <c r="BX34" s="4">
         <v>1</v>
       </c>
     </row>
@@ -11013,7 +10977,7 @@
         <v>1</v>
       </c>
       <c r="U35" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="V35" t="s">
         <v>242</v>
@@ -11031,7 +10995,7 @@
         <v>1</v>
       </c>
       <c r="BI35" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="BJ35" t="s">
         <v>1184</v>
@@ -11040,7 +11004,7 @@
         <v>1</v>
       </c>
       <c r="BM35" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="BN35" t="s">
         <v>1218</v>
@@ -11049,7 +11013,7 @@
         <v>1</v>
       </c>
       <c r="BQ35" s="2" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="BR35" s="2" t="s">
         <v>1099</v>
@@ -11060,16 +11024,16 @@
       <c r="BT35">
         <v>1</v>
       </c>
-      <c r="BU35" t="s">
-        <v>1344</v>
-      </c>
-      <c r="BV35" t="s">
+      <c r="BU35" s="6" t="s">
+        <v>1343</v>
+      </c>
+      <c r="BV35" s="6" t="s">
         <v>939</v>
       </c>
       <c r="BW35">
         <v>3</v>
       </c>
-      <c r="BX35" s="3">
+      <c r="BX35" s="4">
         <v>1</v>
       </c>
     </row>
@@ -11102,7 +11066,7 @@
         <v>1</v>
       </c>
       <c r="BI36" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="BJ36" t="s">
         <v>1185</v>
@@ -11111,7 +11075,7 @@
         <v>1</v>
       </c>
       <c r="BM36" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="BN36" t="s">
         <v>994</v>
@@ -11120,7 +11084,7 @@
         <v>1</v>
       </c>
       <c r="BQ36" s="2" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="BR36" s="2" t="s">
         <v>1100</v>
@@ -11131,16 +11095,16 @@
       <c r="BT36">
         <v>1</v>
       </c>
-      <c r="BU36" t="s">
-        <v>1347</v>
-      </c>
-      <c r="BV36" t="s">
+      <c r="BU36" s="6" t="s">
+        <v>1346</v>
+      </c>
+      <c r="BV36" s="6" t="s">
         <v>940</v>
       </c>
       <c r="BW36">
         <v>3</v>
       </c>
-      <c r="BX36" s="3">
+      <c r="BX36" s="4">
         <v>1</v>
       </c>
     </row>
@@ -11164,7 +11128,7 @@
         <v>1</v>
       </c>
       <c r="BI37" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="BJ37" t="s">
         <v>1193</v>
@@ -11173,7 +11137,7 @@
         <v>1</v>
       </c>
       <c r="BM37" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="BN37" t="s">
         <v>994</v>
@@ -11182,7 +11146,7 @@
         <v>1</v>
       </c>
       <c r="BQ37" s="2" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="BR37" s="2" t="s">
         <v>1099</v>
@@ -11194,7 +11158,7 @@
         <v>1</v>
       </c>
       <c r="BU37" s="2" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="BV37" s="2" t="s">
         <v>941</v>
@@ -11229,7 +11193,7 @@
         <v>1</v>
       </c>
       <c r="BI38" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="BJ38" t="s">
         <v>1194</v>
@@ -11238,7 +11202,7 @@
         <v>1</v>
       </c>
       <c r="BM38" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="BN38" t="s">
         <v>994</v>
@@ -11247,7 +11211,7 @@
         <v>1</v>
       </c>
       <c r="BQ38" s="2" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="BR38" s="2" t="s">
         <v>1101</v>
@@ -11259,7 +11223,7 @@
         <v>1</v>
       </c>
       <c r="BU38" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="BV38" t="s">
         <v>942</v>
@@ -11294,7 +11258,7 @@
         <v>1</v>
       </c>
       <c r="BI39" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="BJ39" t="s">
         <v>1195</v>
@@ -11303,7 +11267,7 @@
         <v>1</v>
       </c>
       <c r="BM39" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="BN39" t="s">
         <v>994</v>
@@ -11312,7 +11276,7 @@
         <v>1</v>
       </c>
       <c r="BQ39" s="2" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="BR39" s="2" t="s">
         <v>1102</v>
@@ -11324,7 +11288,7 @@
         <v>1</v>
       </c>
       <c r="BU39" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="BV39" t="s">
         <v>946</v>
@@ -11356,7 +11320,7 @@
         <v>1</v>
       </c>
       <c r="BI40" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="BJ40" t="s">
         <v>1196</v>
@@ -11365,7 +11329,7 @@
         <v>1</v>
       </c>
       <c r="BM40" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="BN40" t="s">
         <v>994</v>
@@ -11374,7 +11338,7 @@
         <v>1</v>
       </c>
       <c r="BQ40" s="2" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="BR40" s="2" t="s">
         <v>1097</v>
@@ -11386,7 +11350,7 @@
         <v>1</v>
       </c>
       <c r="BU40" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="BV40" t="s">
         <v>944</v>
@@ -11396,17 +11360,20 @@
       </c>
     </row>
     <row r="41" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
       <c r="U41" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="V41" t="s">
         <v>225</v>
@@ -11415,7 +11382,7 @@
         <v>1</v>
       </c>
       <c r="BI41" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="BJ41" t="s">
         <v>1197</v>
@@ -11424,7 +11391,7 @@
         <v>1</v>
       </c>
       <c r="BM41" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="BN41" t="s">
         <v>994</v>
@@ -11433,7 +11400,7 @@
         <v>1</v>
       </c>
       <c r="BQ41" s="2" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="BR41" s="2" t="s">
         <v>1104</v>
@@ -11445,7 +11412,7 @@
         <v>1</v>
       </c>
       <c r="BU41" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="BV41" t="s">
         <v>947</v>
@@ -11465,7 +11432,7 @@
         <v>1</v>
       </c>
       <c r="U42" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="V42" t="s">
         <v>226</v>
@@ -11474,7 +11441,7 @@
         <v>1</v>
       </c>
       <c r="BI42" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="BJ42" t="s">
         <v>1198</v>
@@ -11483,7 +11450,7 @@
         <v>1</v>
       </c>
       <c r="BM42" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="BN42" t="s">
         <v>994</v>
@@ -11492,7 +11459,7 @@
         <v>1</v>
       </c>
       <c r="BQ42" s="2" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="BR42" s="2" t="s">
         <v>1105</v>
@@ -11503,16 +11470,16 @@
       <c r="BT42">
         <v>1</v>
       </c>
-      <c r="BU42" t="s">
-        <v>1375</v>
-      </c>
-      <c r="BV42" t="s">
+      <c r="BU42" s="6" t="s">
+        <v>1374</v>
+      </c>
+      <c r="BV42" s="6" t="s">
         <v>943</v>
       </c>
       <c r="BW42">
         <v>3</v>
       </c>
-      <c r="BX42" s="3">
+      <c r="BX42" s="4">
         <v>1</v>
       </c>
     </row>
@@ -11527,7 +11494,7 @@
         <v>1</v>
       </c>
       <c r="U43" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="V43" t="s">
         <v>227</v>
@@ -11548,7 +11515,7 @@
         <v>1</v>
       </c>
       <c r="BM43" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="BN43" t="s">
         <v>994</v>
@@ -11557,7 +11524,7 @@
         <v>1</v>
       </c>
       <c r="BQ43" s="2" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="BR43" s="2" t="s">
         <v>1106</v>
@@ -11569,7 +11536,7 @@
         <v>1</v>
       </c>
       <c r="BU43" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="BV43" t="s">
         <v>945</v>
@@ -11613,7 +11580,7 @@
         <v>1</v>
       </c>
       <c r="BM44" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="BN44" t="s">
         <v>994</v>
@@ -11622,7 +11589,7 @@
         <v>1</v>
       </c>
       <c r="BQ44" s="2" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="BR44" s="2" t="s">
         <v>1107</v>
@@ -11634,7 +11601,7 @@
         <v>1</v>
       </c>
       <c r="BU44" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="BV44" t="s">
         <v>953</v>
@@ -11675,7 +11642,7 @@
         <v>1</v>
       </c>
       <c r="BM45" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="BN45" t="s">
         <v>994</v>
@@ -11684,7 +11651,7 @@
         <v>1</v>
       </c>
       <c r="BQ45" s="2" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="BR45" s="2" t="s">
         <v>1108</v>
@@ -11696,7 +11663,7 @@
         <v>1</v>
       </c>
       <c r="BU45" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="BV45" t="s">
         <v>951</v>
@@ -11740,7 +11707,7 @@
         <v>1</v>
       </c>
       <c r="BM46" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="BN46" t="s">
         <v>994</v>
@@ -11749,7 +11716,7 @@
         <v>1</v>
       </c>
       <c r="BQ46" s="2" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="BR46" s="2" t="s">
         <v>1109</v>
@@ -11761,7 +11728,7 @@
         <v>1</v>
       </c>
       <c r="BU46" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="BV46" t="s">
         <v>952</v>
@@ -11781,7 +11748,7 @@
         <v>1</v>
       </c>
       <c r="U47" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="V47" t="s">
         <v>228</v>
@@ -11790,7 +11757,7 @@
         <v>1</v>
       </c>
       <c r="BI47" s="2" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="BJ47" s="2" t="s">
         <v>1151</v>
@@ -11802,7 +11769,7 @@
         <v>1</v>
       </c>
       <c r="BM47" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="BN47" t="s">
         <v>994</v>
@@ -11811,7 +11778,7 @@
         <v>1</v>
       </c>
       <c r="BQ47" s="2" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="BR47" s="2" t="s">
         <v>1111</v>
@@ -11823,7 +11790,7 @@
         <v>1</v>
       </c>
       <c r="BU47" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="BV47" t="s">
         <v>948</v>
@@ -11843,7 +11810,7 @@
         <v>1</v>
       </c>
       <c r="U48" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="V48" t="s">
         <v>229</v>
@@ -11852,7 +11819,7 @@
         <v>1</v>
       </c>
       <c r="BI48" s="2" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="BJ48" s="2" t="s">
         <v>1152</v>
@@ -11864,7 +11831,7 @@
         <v>1</v>
       </c>
       <c r="BM48" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="BN48" t="s">
         <v>994</v>
@@ -11873,7 +11840,7 @@
         <v>1</v>
       </c>
       <c r="BQ48" s="2" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="BR48" s="2" t="s">
         <v>1112</v>
@@ -11885,7 +11852,7 @@
         <v>1</v>
       </c>
       <c r="BU48" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="BV48" t="s">
         <v>950</v>
@@ -11914,7 +11881,7 @@
         <v>1</v>
       </c>
       <c r="BI49" s="2" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="BJ49" s="2" t="s">
         <v>1153</v>
@@ -11926,7 +11893,7 @@
         <v>1</v>
       </c>
       <c r="BQ49" s="2" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="BR49" s="2" t="s">
         <v>1113</v>
@@ -11938,7 +11905,7 @@
         <v>1</v>
       </c>
       <c r="BU49" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="BV49" t="s">
         <v>949</v>
@@ -11967,7 +11934,7 @@
         <v>1</v>
       </c>
       <c r="BI50" s="2" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="BJ50" s="2" t="s">
         <v>1155</v>
@@ -11979,7 +11946,7 @@
         <v>1</v>
       </c>
       <c r="BQ50" s="2" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="BR50" s="2" t="s">
         <v>1114</v>
@@ -11991,7 +11958,7 @@
         <v>1</v>
       </c>
       <c r="BU50" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="BV50" t="s">
         <v>957</v>
@@ -12020,7 +11987,7 @@
         <v>1</v>
       </c>
       <c r="BI51" s="2" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="BJ51" s="2" t="s">
         <v>1156</v>
@@ -12032,7 +11999,7 @@
         <v>1</v>
       </c>
       <c r="BQ51" s="2" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="BR51" s="2" t="s">
         <v>1115</v>
@@ -12044,7 +12011,7 @@
         <v>1</v>
       </c>
       <c r="BU51" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="BV51" t="s">
         <v>956</v>
@@ -12067,7 +12034,7 @@
         <v>1</v>
       </c>
       <c r="BI52" s="2" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="BJ52" s="2" t="s">
         <v>1163</v>
@@ -12079,7 +12046,7 @@
         <v>1</v>
       </c>
       <c r="BQ52" s="2" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="BR52" s="2" t="s">
         <v>1117</v>
@@ -12091,7 +12058,7 @@
         <v>1</v>
       </c>
       <c r="BU52" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="BV52" t="s">
         <v>955</v>
@@ -12111,7 +12078,7 @@
         <v>1</v>
       </c>
       <c r="BI53" s="2" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="BJ53" s="2" t="s">
         <v>1165</v>
@@ -12123,7 +12090,7 @@
         <v>1</v>
       </c>
       <c r="BQ53" s="2" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="BR53" s="2" t="s">
         <v>1118</v>
@@ -12135,7 +12102,7 @@
         <v>1</v>
       </c>
       <c r="BU53" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="BV53" t="s">
         <v>954</v>
@@ -12146,7 +12113,7 @@
     </row>
     <row r="54" spans="1:75" x14ac:dyDescent="0.25">
       <c r="BI54" s="2" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="BJ54" s="2" t="s">
         <v>1144</v>
@@ -12158,7 +12125,7 @@
         <v>1</v>
       </c>
       <c r="BQ54" s="2" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="BR54" s="2" t="s">
         <v>1119</v>
@@ -12170,7 +12137,7 @@
         <v>1</v>
       </c>
       <c r="BU54" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="BV54" t="s">
         <v>959</v>
@@ -12181,7 +12148,7 @@
     </row>
     <row r="55" spans="1:75" x14ac:dyDescent="0.25">
       <c r="BI55" s="2" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="BJ55" s="2" t="s">
         <v>1174</v>
@@ -12193,7 +12160,7 @@
         <v>1</v>
       </c>
       <c r="BQ55" s="2" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="BR55" s="2" t="s">
         <v>1120</v>
@@ -12205,7 +12172,7 @@
         <v>1</v>
       </c>
       <c r="BU55" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="BV55" t="s">
         <v>958</v>
@@ -12216,7 +12183,7 @@
     </row>
     <row r="56" spans="1:75" x14ac:dyDescent="0.25">
       <c r="BI56" s="2" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="BJ56" s="2" t="s">
         <v>1178</v>
@@ -12228,7 +12195,7 @@
         <v>1</v>
       </c>
       <c r="BQ56" s="2" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="BR56" s="2" t="s">
         <v>1122</v>
@@ -12242,7 +12209,7 @@
     </row>
     <row r="57" spans="1:75" x14ac:dyDescent="0.25">
       <c r="BI57" s="2" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="BJ57" s="2" t="s">
         <v>1179</v>
@@ -12254,7 +12221,7 @@
         <v>1</v>
       </c>
       <c r="BQ57" s="2" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="BR57" s="2" t="s">
         <v>1123</v>
@@ -12268,7 +12235,7 @@
     </row>
     <row r="58" spans="1:75" x14ac:dyDescent="0.25">
       <c r="BQ58" s="2" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="BR58" s="2" t="s">
         <v>1124</v>
@@ -12282,7 +12249,7 @@
     </row>
     <row r="59" spans="1:75" x14ac:dyDescent="0.25">
       <c r="BQ59" s="2" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="BR59" s="2" t="s">
         <v>1125</v>
@@ -12296,7 +12263,7 @@
     </row>
     <row r="60" spans="1:75" x14ac:dyDescent="0.25">
       <c r="BQ60" s="2" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="BR60" s="2" t="s">
         <v>1126</v>
@@ -12310,7 +12277,7 @@
     </row>
     <row r="61" spans="1:75" x14ac:dyDescent="0.25">
       <c r="BQ61" s="2" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="BR61" s="2" t="s">
         <v>1127</v>
@@ -12324,7 +12291,7 @@
     </row>
     <row r="62" spans="1:75" x14ac:dyDescent="0.25">
       <c r="BQ62" s="2" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="BR62" s="2" t="s">
         <v>1128</v>
@@ -12341,42 +12308,42 @@
     <sortCondition ref="AO2:AO15"/>
   </sortState>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="containsText" dxfId="18" priority="1" stopIfTrue="1" operator="containsText" text="Tea Leaves">
+    <cfRule type="containsText" dxfId="9" priority="1" stopIfTrue="1" operator="containsText" text="Tea Leaves">
       <formula>NOT(ISERROR(SEARCH("Tea Leaves",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="2" stopIfTrue="1" operator="containsText" text="Tapioca">
+    <cfRule type="containsText" dxfId="8" priority="2" stopIfTrue="1" operator="containsText" text="Tapioca">
       <formula>NOT(ISERROR(SEARCH("Tapioca",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="3" stopIfTrue="1" operator="containsText" text="Starfruit">
+    <cfRule type="containsText" dxfId="7" priority="3" stopIfTrue="1" operator="containsText" text="Starfruit">
       <formula>NOT(ISERROR(SEARCH("Starfruit",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="8" stopIfTrue="1" operator="containsText" text="SnowCicle">
+    <cfRule type="containsText" dxfId="6" priority="8" stopIfTrue="1" operator="containsText" text="SnowCicle">
       <formula>NOT(ISERROR(SEARCH("SnowCicle",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="9" stopIfTrue="1" operator="containsText" text="Bubble">
+    <cfRule type="containsText" dxfId="5" priority="9" stopIfTrue="1" operator="containsText" text="Bubble">
       <formula>NOT(ISERROR(SEARCH("Bubble",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="12" stopIfTrue="1" operator="containsText" text="Moon Cheese">
+    <cfRule type="containsText" dxfId="4" priority="12" stopIfTrue="1" operator="containsText" text="Moon Cheese">
       <formula>NOT(ISERROR(SEARCH("Moon Cheese",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R1048576">
-    <cfRule type="containsText" dxfId="12" priority="16" stopIfTrue="1" operator="containsText" text=" + ">
+    <cfRule type="containsText" dxfId="3" priority="16" stopIfTrue="1" operator="containsText" text=" + ">
       <formula>NOT(ISERROR(SEARCH(" + ",R1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="containsText" dxfId="11" priority="15" stopIfTrue="1" operator="containsText" text=" + ">
+    <cfRule type="containsText" dxfId="2" priority="15" stopIfTrue="1" operator="containsText" text=" + ">
       <formula>NOT(ISERROR(SEARCH(" + ",V1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:Z1048576">
-    <cfRule type="containsText" dxfId="10" priority="14" stopIfTrue="1" operator="containsText" text=" + ">
+    <cfRule type="containsText" dxfId="1" priority="14" stopIfTrue="1" operator="containsText" text=" + ">
       <formula>NOT(ISERROR(SEARCH(" + ",Z1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD1:AD1048576">
-    <cfRule type="containsText" dxfId="9" priority="13" stopIfTrue="1" operator="containsText" text=" + ">
+    <cfRule type="containsText" dxfId="0" priority="13" stopIfTrue="1" operator="containsText" text=" + ">
       <formula>NOT(ISERROR(SEARCH(" + ",AD1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12386,10 +12353,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D86D7E6B-F615-4EC2-9ABB-4F66E247620A}">
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A23"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12467,6 +12434,11 @@
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>802</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>1533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>